<commit_message>
Add test Excel report with Market Cap and Volume
</commit_message>
<xml_diff>
--- a/reports/2026-01-17.xlsx
+++ b/reports/2026-01-17.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-01-17 19:44 UTC</t>
+          <t>2026-01-17 20:26 UTC</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$740.18M</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.95M</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -691,12 +691,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$394.28M</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.45M</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -737,12 +737,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$597.12M</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.13M</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -783,12 +783,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$365.91M</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.48M</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -829,12 +829,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.15B</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$4.57M</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -875,12 +875,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$753.93M</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$3.47M</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -921,12 +921,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.26B</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.71M</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -967,12 +967,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$505.02M</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.15M</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1013,12 +1013,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$384.17M</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.07M</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -1059,12 +1059,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.69B</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$5.98M</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -1202,12 +1202,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$334.63M</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$14.23M</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -1248,12 +1248,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$131.40M</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$4.31M</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -1294,12 +1294,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$394.28M</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.45M</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -1340,12 +1340,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$981.15M</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.22M</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -1386,12 +1386,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$145.43M</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$3.40M</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -1432,12 +1432,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$955.28M</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$38.78M</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -1478,12 +1478,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$647.58M</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$18.71M</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1524,12 +1524,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.18B</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$9.79M</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1570,12 +1570,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$200.51M</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$8.78M</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -1616,12 +1616,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.03B</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$7.74M</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -1759,12 +1759,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$334.63M</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$14.23M</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -1805,12 +1805,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$131.40M</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$4.31M</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$394.28M</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.45M</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -1897,12 +1897,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$647.58M</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$18.71M</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -1943,12 +1943,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$981.15M</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.22M</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -1989,12 +1989,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$145.43M</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$3.40M</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -2035,12 +2035,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$121.99M</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.78M</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -2081,12 +2081,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$2.92B</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$3.65M</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -2127,12 +2127,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$664.65M</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.09M</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -2173,12 +2173,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$365.91M</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>$1.48M</t>
         </is>
       </c>
       <c r="G11" t="n">

</xml_diff>